<commit_message>
Update tutorial example inputBusOperadorCompleto
</commit_message>
<xml_diff>
--- a/examples/tutorial/InputBusOperadorCompleto.xlsx
+++ b/examples/tutorial/InputBusOperadorCompleto.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ednaruckhaus/Nextcloud/Mapeathor-tutorial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ednaruckhaus/Documents/GitHub/Mapeathor/examples/tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811E3707-FC7A-3743-B7D9-184F8E038512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBF605A-59AE-8646-9361-191360025C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12740" yWindow="3800" windowWidth="22860" windowHeight="15820" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9520" yWindow="460" windowWidth="22860" windowHeight="15820" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
-    <sheet name="Source" sheetId="2" r:id="rId2"/>
-    <sheet name="Subject" sheetId="3" r:id="rId3"/>
-    <sheet name="PredicateObjectMaps" sheetId="4" r:id="rId4"/>
-    <sheet name="Functions" sheetId="5" r:id="rId5"/>
+    <sheet name="Prefix" sheetId="1" r:id="rId1"/>
+    <sheet name="Subject" sheetId="3" r:id="rId2"/>
+    <sheet name="Source" sheetId="2" r:id="rId3"/>
+    <sheet name="Predicate_Object" sheetId="4" r:id="rId4"/>
+    <sheet name="Function" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="76">
   <si>
     <t>Prefix</t>
   </si>
@@ -247,17 +247,23 @@
     <t>tmkosjourney:{direction_id}</t>
   </si>
   <si>
-    <t>recurso-autobus:operador/{agency_id}</t>
-  </si>
-  <si>
-    <t>recurso-autobus:ruta/{route_id}</t>
+    <t>http://vocab.ciudadesabiertas.es/recurso/transporte/autobus/linea/{line_id}</t>
+  </si>
+  <si>
+    <t>http://vocab.ciudadesabiertas.es/recurso/transporte/autobus/presentacion/pres-{line_id}</t>
+  </si>
+  <si>
+    <t>http://vocab.ciudadesabiertas.es/recurso/transporte/autobus/operador/{agency_id}</t>
+  </si>
+  <si>
+    <t>http://vocab.ciudadesabiertas.es/recurso/transporte/autobus/ruta/{route_id}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -281,6 +287,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -299,10 +313,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -318,8 +333,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -635,7 +652,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,8 +722,86 @@
       <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="9" t="s">
         <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{8E430F34-326D-2C4F-9F44-5760B2C7F73F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -834,87 +929,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B22" sqref="B21:B22"/>
+    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1144,6 +1164,9 @@
       <c r="C13" t="s">
         <v>67</v>
       </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1197,7 +1220,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1212,10 +1237,10 @@
         <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tutorial example csv files and mappings
</commit_message>
<xml_diff>
--- a/examples/tutorial/InputBusOperadorCompleto.xlsx
+++ b/examples/tutorial/InputBusOperadorCompleto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ednaruckhaus/Documents/GitHub/Mapeathor/examples/tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB820F20-B103-5D46-A3CB-63BDCA701A43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11571A57-762E-A145-A7C1-1FE9903CFAB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14420" yWindow="460" windowWidth="22860" windowHeight="15820" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14420" yWindow="460" windowWidth="22860" windowHeight="15820" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" r:id="rId1"/>
@@ -133,9 +133,6 @@
     <t>idLine</t>
   </si>
   <si>
-    <t>examples/publicBus/routes.csv</t>
-  </si>
-  <si>
     <t>tmjourney:Line</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
     <t>idRoute</t>
   </si>
   <si>
-    <t>examples/publicBus/operator-lines.csv</t>
-  </si>
-  <si>
     <t>tmjourney:Route</t>
   </si>
   <si>
@@ -254,6 +248,12 @@
   </si>
   <si>
     <t>{route_line}</t>
+  </si>
+  <si>
+    <t>examples/tutorial/operator-lines.csv</t>
+  </si>
+  <si>
+    <t>examples/tutorial/routes.csv</t>
   </si>
 </sst>
 </file>
@@ -717,10 +717,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -765,7 +765,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -781,18 +781,18 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -803,18 +803,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -825,18 +825,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -881,43 +881,43 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
         <v>48</v>
       </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -974,7 +974,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -985,10 +985,10 @@
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -999,10 +999,10 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -1016,10 +1016,10 @@
         <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
@@ -1036,13 +1036,13 @@
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s">
         <v>33</v>
@@ -1050,17 +1050,17 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="3"/>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G7" t="s">
         <v>33</v>
@@ -1068,10 +1068,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -1086,15 +1086,15 @@
         <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -1106,7 +1106,7 @@
         <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1114,55 +1114,55 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1170,13 +1170,13 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1184,27 +1184,27 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1217,7 +1217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update tutorial input spreadsheet
</commit_message>
<xml_diff>
--- a/examples/tutorial/InputBusOperadorCompleto.xlsx
+++ b/examples/tutorial/InputBusOperadorCompleto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ednaruckhaus/Documents/GitHub/Mapeathor/examples/tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11571A57-762E-A145-A7C1-1FE9903CFAB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E285E9-6FDC-C043-8468-128D1EC75BB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14420" yWindow="460" windowWidth="22860" windowHeight="15820" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14420" yWindow="460" windowWidth="22860" windowHeight="15820" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" r:id="rId1"/>
@@ -736,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -855,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>